<commit_message>
updated analyses and data
to further anonymise data
</commit_message>
<xml_diff>
--- a/data/results of data sharing requests - blinded and shuffled.xlsx
+++ b/data/results of data sharing requests - blinded and shuffled.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/irap-data-availability/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian-Hussey/git/irap-data-availability/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8C488A-4A9F-D34E-A586-A1764F5E4EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B012803E-0534-8341-B78F-12C690D5E185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="147">
-  <si>
-    <t>Journal of Contextual Behavioral Science</t>
-  </si>
-  <si>
-    <t>The Psychological Record</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="134">
   <si>
     <t>E5RG8PK6</t>
   </si>
@@ -48,48 +42,21 @@
     <t>KVU2FMQ5</t>
   </si>
   <si>
-    <t>International Journal of Psychology &amp; Psychological Therapy</t>
-  </si>
-  <si>
     <t>UDNNYRXA</t>
   </si>
   <si>
-    <t>Frontiers in Psychology</t>
-  </si>
-  <si>
-    <t>Journal of Behavior Therapy and Experimental Psychiatry</t>
-  </si>
-  <si>
-    <t>Behavior and Social Issues</t>
-  </si>
-  <si>
-    <t>Emotional &amp; Behavioural Difficulties</t>
-  </si>
-  <si>
     <t>GPHKN3IR</t>
   </si>
   <si>
-    <t>Behavioural Processes</t>
-  </si>
-  <si>
     <t>6275MA6V</t>
   </si>
   <si>
-    <t>Motivation and Emotion</t>
-  </si>
-  <si>
     <t>AGZTLUCT</t>
   </si>
   <si>
-    <t>Dementia: The International Journal of Social Research and Practice</t>
-  </si>
-  <si>
     <t>AM4KK3J3</t>
   </si>
   <si>
-    <t>Journal of Eating Disorders</t>
-  </si>
-  <si>
     <t>PYADQXZL</t>
   </si>
   <si>
@@ -192,9 +159,6 @@
     <t>6C8DT2HT</t>
   </si>
   <si>
-    <t>Social Psychology of Education: An International Journal</t>
-  </si>
-  <si>
     <t>UXKIDUYY</t>
   </si>
   <si>
@@ -223,9 +187,6 @@
   </si>
   <si>
     <t>D6JNLGEF</t>
-  </si>
-  <si>
-    <t>International Journal of Environmental Research and Public Health</t>
   </si>
   <si>
     <t>year</t>
@@ -1374,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F9036-BD7F-8941-AAC0-FD3B8EC13872}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="119" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1398,84 +1359,84 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="N1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3">
         <v>2019</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J2" s="5">
         <v>44995</v>
@@ -1490,45 +1451,45 @@
         <v>0</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="O2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3">
         <v>2019</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J3" s="5">
         <v>44995</v>
@@ -1543,45 +1504,45 @@
         <v>0</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="O3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C4" s="3">
         <v>2022</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J4" s="5">
         <v>44995</v>
@@ -1596,45 +1557,45 @@
         <v>1</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="P4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3">
         <v>2022</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J5" s="5">
         <v>44995</v>
@@ -1649,45 +1610,45 @@
         <v>0</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="P5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C6" s="3">
         <v>2020</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J6" s="5">
         <v>45005</v>
@@ -1702,45 +1663,45 @@
         <v>0</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="O6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C7" s="3">
         <v>2019</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J7" s="5">
         <v>45005</v>
@@ -1759,39 +1720,39 @@
         <v>0</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3">
         <v>2020</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J8" s="5">
         <v>44995</v>
@@ -1806,45 +1767,45 @@
         <v>0</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="O8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C9" s="3">
         <v>2018</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J9" s="5">
         <v>44999</v>
@@ -1863,39 +1824,39 @@
         <v>0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3">
         <v>2021</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J10" s="5">
         <v>45013</v>
@@ -1914,39 +1875,39 @@
         <v>0</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C11" s="3">
         <v>2018</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J11" s="5">
         <v>44995</v>
@@ -1961,45 +1922,45 @@
         <v>0</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="O11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C12" s="3">
         <v>2021</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J12" s="5">
         <v>45013</v>
@@ -2015,42 +1976,42 @@
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="P12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C13" s="3">
         <v>2019</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J13" s="5">
         <v>45006</v>
@@ -2065,45 +2026,45 @@
         <v>0</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="O13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C14" s="3">
         <v>2020</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J14" s="5">
         <v>45005</v>
@@ -2118,45 +2079,45 @@
         <v>0</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="O14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C15" s="3">
         <v>2019</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J15" s="5">
         <v>45006</v>
@@ -2171,45 +2132,45 @@
         <v>1</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="P15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C16" s="3">
         <v>2020</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J16" s="5">
         <v>45006</v>
@@ -2224,45 +2185,45 @@
         <v>0</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="O16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C17" s="3">
         <v>2020</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J17" s="5">
         <v>44995</v>
@@ -2281,40 +2242,40 @@
         <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C18" s="3">
         <v>2021</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J18" s="5">
         <v>44995</v>
@@ -2329,46 +2290,46 @@
         <v>0</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="P18" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C19" s="3">
         <v>2021</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J19" s="5">
         <v>44995</v>
@@ -2383,46 +2344,46 @@
         <v>0</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="O19" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3">
         <v>2022</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J20" s="5">
         <v>44999</v>
@@ -2437,46 +2398,46 @@
         <v>0</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="P20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3">
         <v>2020</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J21" s="5">
         <v>44995</v>
@@ -2491,46 +2452,46 @@
         <v>0</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="P21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3">
         <v>2019</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J22" s="5">
         <v>45013</v>
@@ -2545,45 +2506,45 @@
         <v>0</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="O22" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C23" s="3">
         <v>2021</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J23" s="5">
         <v>44995</v>
@@ -2598,45 +2559,45 @@
         <v>0</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="P23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C24" s="3">
         <v>2018</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J24" s="5">
         <v>44999</v>
@@ -2651,45 +2612,45 @@
         <v>0</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="O24" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C25" s="3">
         <v>2021</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J25" s="5">
         <v>44995</v>
@@ -2708,39 +2669,39 @@
         <v>0</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C26" s="3">
         <v>2022</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J26" s="5">
         <v>44995</v>
@@ -2755,45 +2716,45 @@
         <v>0</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="P26" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C27" s="3">
         <v>2019</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J27" s="5">
         <v>45013</v>
@@ -2808,45 +2769,45 @@
         <v>1</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="O27" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C28" s="3">
         <v>2021</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J28" s="5">
         <v>44995</v>
@@ -2862,42 +2823,42 @@
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="P28" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C29" s="6">
         <v>2018</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J29" s="5">
         <v>45008</v>
@@ -2912,45 +2873,45 @@
         <v>0</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="O29" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C30" s="3">
         <v>2019</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J30" s="5">
         <v>44995</v>
@@ -2965,45 +2926,45 @@
         <v>0</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="P30" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C31" s="3">
         <v>2021</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J31" s="5">
         <v>45006</v>
@@ -3018,45 +2979,45 @@
         <v>0</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="P31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C32" s="3">
         <v>2019</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J32" s="5">
         <v>44995</v>
@@ -3071,45 +3032,45 @@
         <v>0</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="O32" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C33" s="3">
         <v>2022</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J33" s="5">
         <v>45008</v>
@@ -3124,45 +3085,45 @@
         <v>0</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="P33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C34" s="3">
         <v>2020</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J34" s="5">
         <v>45013</v>
@@ -3177,45 +3138,45 @@
         <v>1</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="P34" s="3" t="b">
         <v>1</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C35" s="3">
         <v>2018</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J35" s="5">
         <v>44995</v>
@@ -3230,45 +3191,45 @@
         <v>0</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="O35" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C36" s="3">
         <v>2019</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J36" s="5">
         <v>44995</v>
@@ -3283,45 +3244,45 @@
         <v>0</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="O36" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C37" s="3">
         <v>2020</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J37" s="5">
         <v>44995</v>
@@ -3336,45 +3297,45 @@
         <v>1</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="O37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C38" s="3">
         <v>2019</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J38" s="5">
         <v>45006</v>
@@ -3389,45 +3350,45 @@
         <v>0</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="O38" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C39" s="3">
         <v>2020</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J39" s="5">
         <v>44995</v>
@@ -3442,45 +3403,45 @@
         <v>1</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="O39" s="3" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C40" s="3">
         <v>2019</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J40" s="5">
         <v>45006</v>
@@ -3495,45 +3456,45 @@
         <v>1</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="O40" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="187" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C41" s="3">
         <v>2022</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J41" s="5">
         <v>45013</v>
@@ -3548,45 +3509,45 @@
         <v>0</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="P41" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C42" s="3">
         <v>2019</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J42" s="5">
         <v>44995</v>
@@ -3605,39 +3566,39 @@
         <v>0</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C43" s="3">
         <v>2020</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J43" s="5">
         <v>44995</v>
@@ -3652,45 +3613,45 @@
         <v>0</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="P43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C44" s="3">
         <v>2020</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J44" s="5">
         <v>44995</v>
@@ -3705,45 +3666,45 @@
         <v>1</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="O44" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C45" s="3">
         <v>2020</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J45" s="5">
         <v>45006</v>
@@ -3758,45 +3719,45 @@
         <v>1</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="P45" s="3" t="b">
         <v>1</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C46" s="3">
         <v>2020</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J46" s="5">
         <v>44999</v>
@@ -3811,45 +3772,45 @@
         <v>0</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="O46" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C47" s="3">
         <v>2018</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J47" s="5">
         <v>44995</v>
@@ -3864,45 +3825,45 @@
         <v>0</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="O47" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C48" s="3">
         <v>2021</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J48" s="5">
         <v>44995</v>
@@ -3917,45 +3878,45 @@
         <v>1</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="P48" s="3" t="b">
         <v>1</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C49" s="3">
         <v>2020</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J49" s="5">
         <v>44995</v>
@@ -3970,45 +3931,45 @@
         <v>1</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="O49" s="4" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="P49" s="3" t="b">
         <v>1</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C50" s="3">
         <v>2020</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J50" s="5">
         <v>44999</v>
@@ -4023,45 +3984,45 @@
         <v>0</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="O50" s="4" t="b">
         <v>0</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C51" s="3">
         <v>2019</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J51" s="5">
         <v>45007</v>
@@ -4076,45 +4037,45 @@
         <v>0</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="P51" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C52" s="3">
         <v>2019</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J52" s="5">
         <v>44995</v>
@@ -4129,45 +4090,45 @@
         <v>0</v>
       </c>
       <c r="N52" s="8" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="P52" s="3" t="b">
         <v>0</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C53" s="3">
         <v>2018</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="J53" s="5">
         <v>44995</v>
@@ -4186,10 +4147,10 @@
         <v>0</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>